<commit_message>
Add QC results from HTG app for miRNA Repro data
</commit_message>
<xml_diff>
--- a/Paper1/miRNA_Repro_QC_result.xlsx
+++ b/Paper1/miRNA_Repro_QC_result.xlsx
@@ -1,18 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr date1904="false"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Classes\Dissertation\Paper1\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12240" windowHeight="5568"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="52">
   <si>
     <t>Sample Name</t>
   </si>
@@ -174,8 +181,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -211,6 +217,15 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -493,13 +508,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="1"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.44140625" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" customWidth="1"/>
+    <col min="3" max="3" width="12.5546875" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" customWidth="1"/>
+    <col min="5" max="5" width="11.77734375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -516,7 +538,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -533,7 +555,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -550,7 +572,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -567,7 +589,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -584,7 +606,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -601,7 +623,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -618,7 +640,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -635,7 +657,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -652,7 +674,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -669,7 +691,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -686,7 +708,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -703,7 +725,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -720,7 +742,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>39</v>
       </c>
@@ -737,7 +759,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>42</v>
       </c>
@@ -754,7 +776,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>45</v>
       </c>
@@ -771,7 +793,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>48</v>
       </c>
@@ -788,7 +810,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>50</v>
       </c>
@@ -807,6 +829,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>